<commit_message>
WP excel spreadsheet - done
</commit_message>
<xml_diff>
--- a/DB/WP.xlsx
+++ b/DB/WP.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="225" windowWidth="13395" windowHeight="11700" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="225" windowWidth="13395" windowHeight="11700"/>
   </bookViews>
   <sheets>
-    <sheet name="node-f1" sheetId="1" r:id="rId1"/>
+    <sheet name="nodes" sheetId="1" r:id="rId1"/>
     <sheet name="node-f2" sheetId="4" r:id="rId2"/>
     <sheet name="neighbor" sheetId="2" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId4"/>
@@ -742,8 +742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF73"/>
   <sheetViews>
-    <sheetView topLeftCell="I27" workbookViewId="0">
-      <selection activeCell="AE3" sqref="AE3:AF51"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:K73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6571,8 +6571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="F92" sqref="F92:F118"/>
+    <sheetView topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
combined floors - mapping on an individual floor will not work right now (removed for testing between floors)
</commit_message>
<xml_diff>
--- a/DB/WP.xlsx
+++ b/DB/WP.xlsx
@@ -10,14 +10,15 @@
     <sheet name="nodes" sheetId="1" r:id="rId1"/>
     <sheet name="node-f2" sheetId="4" r:id="rId2"/>
     <sheet name="neighbor" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId4"/>
+    <sheet name="interfloor" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="126">
   <si>
     <t>nID</t>
   </si>
@@ -389,6 +390,12 @@
   </si>
   <si>
     <t>F2-CL1</t>
+  </si>
+  <si>
+    <t>INSERT INTO tblInterFloor VALUES (</t>
+  </si>
+  <si>
+    <t>[F1-RN - Walk-In Clinic, F1-C1_4 - Walk-In Clinic, F1-E1 - Walk-In Clinic, F1-C1_2 - Walk-In Clinic, F1-C1_3 - Walk-In Clinic, F1-C1_1 - Walk-In Clinic, F1-RX - Walk-In Clinic, F1-E2 - Walk-In Clinic, F1-C1_0 - Walk-In Clinic, F1-108 - Walk-In Clinic, F1-108_0 - Walk-In Clinic, F1-108R - Walk-In Clinic, F1-108_1 - Walk-In Clinic, F1-108_2 - Walk-In Clinic, F1-C2_0 - Walk-In Clinic, F1-108A_0 - Walk-In Clinic, F1-108A_1 - Walk-In Clinic, F1-108A_2 - Walk-In Clinic, F1-108P - Walk-In Clinic, F1-108C - Walk-In Clinic, F1-108A_3 - Walk-In Clinic, F1-108B - Walk-In Clinic, F1-T1 - Walk-In Clinic, F1-108O - Walk-In Clinic, F1-108A_4 - Walk-In Clinic, F1-C3_0 - Walk-In Clinic, F1-T2 - Walk-In Clinic, F1-C2_1 - Walk-In Clinic, F1-108D - Walk-In Clinic, F1-108A_5 - Walk-In Clinic, F1-108A_6 - Walk-In Clinic, F1-108A_7 - Walk-In Clinic, F1-S2 - Walk-In Clinic, F2-S2 - Clinical Labs, F1-108A_8 - Walk-In Clinic, F1-108E - Walk-In Clinic, F1-EL - Walk-In Clinic, F2-EL - Clinical Labs, F1-108L - Walk-In Clinic, F1-RS - Walk-In Clinic, F1-108A_9 - Walk-In Clinic, F1-108F - Walk-In Clinic, F1-108J - Walk-In Clinic, F1-108K - Walk-In Clinic, F1-108G - Walk-In Clinic, F2-C1_0 - Clinical Labs, F1-108A_10 - Walk-In Clinic, F1-108I - Walk-In Clinic, F1-108H - Walk-In Clinic, F2-R1 - Clinical Labs, F2-C1_1 - Clinical Labs, F2-XR - Radiology]</t>
   </si>
 </sst>
 </file>
@@ -740,10 +747,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF73"/>
+  <dimension ref="A1:AF75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K73"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51:V51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -894,7 +901,7 @@
         <v>21</v>
       </c>
       <c r="Y3" t="str">
-        <f t="shared" ref="Y3:AA66" si="1">IF(S3&lt;&gt;"",$B3,"")</f>
+        <f t="shared" ref="Y3:Y66" si="1">IF(S3&lt;&gt;"",$B3,"")</f>
         <v>F1-C2_0</v>
       </c>
       <c r="Z3" t="str">
@@ -5048,7 +5055,7 @@
         <v>110</v>
       </c>
       <c r="Y67" t="str">
-        <f t="shared" ref="Y67:AA73" si="10">IF(S67&lt;&gt;"",$B67,"")</f>
+        <f t="shared" ref="Y67:Y73" si="10">IF(S67&lt;&gt;"",$B67,"")</f>
         <v>F2-LAB_E</v>
       </c>
       <c r="Z67" t="str">
@@ -5465,6 +5472,60 @@
       <c r="AF73" t="str">
         <f t="shared" si="17"/>
         <v/>
+      </c>
+    </row>
+    <row r="75" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="S75">
+        <f>COUNTIF(S2:S73,"&lt;&gt;''")</f>
+        <v>72</v>
+      </c>
+      <c r="T75">
+        <f>COUNTIF(T2:T73,"&lt;&gt;")</f>
+        <v>41</v>
+      </c>
+      <c r="U75">
+        <f t="shared" ref="U75:V75" si="18">COUNTIF(U2:U73,"&lt;&gt;")</f>
+        <v>24</v>
+      </c>
+      <c r="V75">
+        <f t="shared" si="18"/>
+        <v>5</v>
+      </c>
+      <c r="W75">
+        <f>SUM(S75:V75)</f>
+        <v>142</v>
+      </c>
+      <c r="Y75">
+        <f>72 - COUNTBLANK(Y2:Y73)</f>
+        <v>72</v>
+      </c>
+      <c r="Z75">
+        <f t="shared" ref="Z75:AF75" si="19">72 - COUNTBLANK(Z2:Z73)</f>
+        <v>72</v>
+      </c>
+      <c r="AA75">
+        <f t="shared" si="19"/>
+        <v>41</v>
+      </c>
+      <c r="AB75">
+        <f t="shared" si="19"/>
+        <v>41</v>
+      </c>
+      <c r="AC75">
+        <f t="shared" si="19"/>
+        <v>24</v>
+      </c>
+      <c r="AD75">
+        <f t="shared" si="19"/>
+        <v>24</v>
+      </c>
+      <c r="AE75">
+        <f t="shared" si="19"/>
+        <v>5</v>
+      </c>
+      <c r="AF75">
+        <f t="shared" si="19"/>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -6569,10 +6630,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F118"/>
+  <dimension ref="A1:F143"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F118"/>
+    <sheetView topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6620,7 +6681,7 @@
         <v>20</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3:F63" si="0">E$1 &amp; A3 &amp; ", '" &amp; B3 &amp; "', '" &amp; C3 &amp; "');"</f>
+        <f t="shared" ref="F3:F66" si="0">E$1 &amp; A3 &amp; ", '" &amp; B3 &amp; "', '" &amp; C3 &amp; "');"</f>
         <v>INSERT INTO tblNeighbors VALUES (2, 'F1-C2_0', 'F1-EL');</v>
       </c>
     </row>
@@ -7535,7 +7596,7 @@
         <v>113</v>
       </c>
       <c r="F64" t="str">
-        <f t="shared" ref="F64:F118" si="1">E$1 &amp; A64 &amp; ", '" &amp; B64 &amp; "', '" &amp; C64 &amp; "');"</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO tblNeighbors VALUES (63, 'F2-LAB_B', 'F2-LAB_A');</v>
       </c>
     </row>
@@ -7550,7 +7611,7 @@
         <v>119</v>
       </c>
       <c r="F65" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>INSERT INTO tblNeighbors VALUES (64, 'F2-LAB_C', 'F2-LAB_B0');</v>
       </c>
     </row>
@@ -7565,7 +7626,7 @@
         <v>119</v>
       </c>
       <c r="F66" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>INSERT INTO tblNeighbors VALUES (65, 'F2-LAB_D', 'F2-LAB_B0');</v>
       </c>
     </row>
@@ -7580,7 +7641,7 @@
         <v>111</v>
       </c>
       <c r="F67" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="F67:F130" si="1">E$1 &amp; A67 &amp; ", '" &amp; B67 &amp; "', '" &amp; C67 &amp; "');"</f>
         <v>INSERT INTO tblNeighbors VALUES (66, 'F2-LAB_E', 'F2-LAB_4');</v>
       </c>
     </row>
@@ -8024,14 +8085,14 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>19</v>
+        <v>62</v>
       </c>
       <c r="C97" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="F97" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tblNeighbors VALUES (96, 'F1-C2_0', 'F1-C1_0');</v>
+        <v>INSERT INTO tblNeighbors VALUES (96, 'F1-108P', 'F1-108P_0');</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
@@ -8039,14 +8100,14 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="C98" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="F98" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tblNeighbors VALUES (97, 'F1-C1_0', 'F1-108');</v>
+        <v>INSERT INTO tblNeighbors VALUES (97, 'F1-108P_0', 'F1-108Q');</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
@@ -8054,14 +8115,14 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>27</v>
+        <v>101</v>
       </c>
       <c r="C99" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="F99" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tblNeighbors VALUES (98, 'F1-C1_2', 'F1-C1_4');</v>
+        <v>INSERT INTO tblNeighbors VALUES (98, 'F2-C1_1', 'F2-C1_0');</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
@@ -8069,14 +8130,14 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>28</v>
+        <v>102</v>
       </c>
       <c r="C100" t="s">
-        <v>31</v>
+        <v>103</v>
       </c>
       <c r="F100" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tblNeighbors VALUES (99, 'F1-C1_3', 'F1-RX');</v>
+        <v>INSERT INTO tblNeighbors VALUES (99, 'F2-C1_0', 'F2-S2');</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
@@ -8084,14 +8145,14 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>29</v>
+        <v>105</v>
       </c>
       <c r="C101" t="s">
-        <v>30</v>
+        <v>107</v>
       </c>
       <c r="F101" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tblNeighbors VALUES (100, 'F1-C1_4', 'F1-RN');</v>
+        <v>INSERT INTO tblNeighbors VALUES (100, 'F2-LAB', 'F2-LAB_0');</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
@@ -8099,14 +8160,14 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>36</v>
+        <v>107</v>
       </c>
       <c r="C102" t="s">
-        <v>37</v>
+        <v>108</v>
       </c>
       <c r="F102" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tblNeighbors VALUES (101, 'F1-108_0', 'F1-108_1');</v>
+        <v>INSERT INTO tblNeighbors VALUES (101, 'F2-LAB_0', 'F2-LAB_1');</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
@@ -8114,14 +8175,14 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>40</v>
+        <v>108</v>
       </c>
       <c r="C103" t="s">
-        <v>50</v>
+        <v>109</v>
       </c>
       <c r="F103" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tblNeighbors VALUES (102, 'F1-108A_0', 'F1-108A_1');</v>
+        <v>INSERT INTO tblNeighbors VALUES (102, 'F2-LAB_1', 'F2-LAB_2');</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
@@ -8129,14 +8190,14 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>50</v>
+        <v>109</v>
       </c>
       <c r="C104" t="s">
-        <v>51</v>
+        <v>110</v>
       </c>
       <c r="F104" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tblNeighbors VALUES (103, 'F1-108A_1', 'F1-108B');</v>
+        <v>INSERT INTO tblNeighbors VALUES (103, 'F2-LAB_2', 'F2-LAB_3');</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
@@ -8144,14 +8205,14 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>41</v>
+        <v>110</v>
       </c>
       <c r="C105" t="s">
-        <v>52</v>
+        <v>117</v>
       </c>
       <c r="F105" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tblNeighbors VALUES (104, 'F1-108A_2', 'F1-108C');</v>
+        <v>INSERT INTO tblNeighbors VALUES (104, 'F2-LAB_3', 'F2-LAB_E');</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
@@ -8159,14 +8220,14 @@
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>42</v>
+        <v>111</v>
       </c>
       <c r="C106" t="s">
-        <v>65</v>
+        <v>112</v>
       </c>
       <c r="F106" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tblNeighbors VALUES (105, 'F1-108A_3', 'F1-T1');</v>
+        <v>INSERT INTO tblNeighbors VALUES (105, 'F2-LAB_4', 'F2-LAB_5');</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
@@ -8174,14 +8235,14 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>43</v>
+        <v>112</v>
       </c>
       <c r="C107" t="s">
-        <v>53</v>
+        <v>113</v>
       </c>
       <c r="F107" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tblNeighbors VALUES (106, 'F1-108A_4', 'F1-108D');</v>
+        <v>INSERT INTO tblNeighbors VALUES (106, 'F2-LAB_5', 'F2-LAB_A');</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
@@ -8189,14 +8250,14 @@
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>44</v>
+        <v>113</v>
       </c>
       <c r="C108" t="s">
-        <v>54</v>
+        <v>114</v>
       </c>
       <c r="F108" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tblNeighbors VALUES (107, 'F1-108A_5', 'F1-108E');</v>
+        <v>INSERT INTO tblNeighbors VALUES (107, 'F2-LAB_A', 'F2-LAB_B');</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
@@ -8204,14 +8265,14 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>45</v>
+        <v>114</v>
       </c>
       <c r="C109" t="s">
-        <v>61</v>
+        <v>119</v>
       </c>
       <c r="F109" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tblNeighbors VALUES (108, 'F1-108A_6', 'F1-108L');</v>
+        <v>INSERT INTO tblNeighbors VALUES (108, 'F2-LAB_B', 'F2-LAB_B0');</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
@@ -8219,14 +8280,14 @@
         <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>46</v>
+        <v>117</v>
       </c>
       <c r="C110" t="s">
-        <v>55</v>
+        <v>110</v>
       </c>
       <c r="F110" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tblNeighbors VALUES (109, 'F1-108A_7', 'F1-108F');</v>
+        <v>INSERT INTO tblNeighbors VALUES (109, 'F2-LAB_E', 'F2-LAB_3');</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
@@ -8234,14 +8295,14 @@
         <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>47</v>
+        <v>118</v>
       </c>
       <c r="C111" t="s">
-        <v>60</v>
+        <v>123</v>
       </c>
       <c r="F111" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tblNeighbors VALUES (110, 'F1-108A_8', 'F1-108K');</v>
+        <v>INSERT INTO tblNeighbors VALUES (110, 'F2-LAB_F', 'F2-CL1');</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
@@ -8249,14 +8310,14 @@
         <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>48</v>
+        <v>119</v>
       </c>
       <c r="C112" t="s">
-        <v>59</v>
+        <v>115</v>
       </c>
       <c r="F112" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tblNeighbors VALUES (111, 'F1-108A_9', 'F1-108J');</v>
+        <v>INSERT INTO tblNeighbors VALUES (111, 'F2-LAB_B0', 'F2-LAB_C');</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
@@ -8264,14 +8325,14 @@
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>49</v>
+        <v>120</v>
       </c>
       <c r="C113" t="s">
-        <v>57</v>
+        <v>121</v>
       </c>
       <c r="F113" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tblNeighbors VALUES (112, 'F1-108A_10', 'F1-108H');</v>
+        <v>INSERT INTO tblNeighbors VALUES (112, 'F2-LAB_R', 'F2-R2');</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
@@ -8279,14 +8340,14 @@
         <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>19</v>
+        <v>121</v>
       </c>
       <c r="C114" t="s">
-        <v>21</v>
+        <v>120</v>
       </c>
       <c r="F114" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tblNeighbors VALUES (113, 'F1-C2_0', 'F1-C2_1');</v>
+        <v>INSERT INTO tblNeighbors VALUES (113, 'F2-R2', 'F2-LAB_R');</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
@@ -8294,14 +8355,14 @@
         <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="C115" t="s">
-        <v>73</v>
+        <v>25</v>
       </c>
       <c r="F115" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tblNeighbors VALUES (114, 'F1-108A_2', 'F1-108O');</v>
+        <v>INSERT INTO tblNeighbors VALUES (114, 'F1-C2_0', 'F1-C1_0');</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
@@ -8309,14 +8370,14 @@
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="C116" t="s">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="F116" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tblNeighbors VALUES (115, 'F1-108A_4', 'F1-T2');</v>
+        <v>INSERT INTO tblNeighbors VALUES (115, 'F1-C1_0', 'F1-108');</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
@@ -8324,14 +8385,14 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="C117" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="F117" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tblNeighbors VALUES (116, 'F1-108A_9', 'F1-108G');</v>
+        <v>INSERT INTO tblNeighbors VALUES (116, 'F1-C1_2', 'F1-C1_4');</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
@@ -8339,14 +8400,389 @@
         <v>117</v>
       </c>
       <c r="B118" t="s">
+        <v>28</v>
+      </c>
+      <c r="C118" t="s">
+        <v>31</v>
+      </c>
+      <c r="F118" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO tblNeighbors VALUES (117, 'F1-C1_3', 'F1-RX');</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>118</v>
+      </c>
+      <c r="B119" t="s">
+        <v>29</v>
+      </c>
+      <c r="C119" t="s">
+        <v>30</v>
+      </c>
+      <c r="F119" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO tblNeighbors VALUES (118, 'F1-C1_4', 'F1-RN');</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>119</v>
+      </c>
+      <c r="B120" t="s">
+        <v>36</v>
+      </c>
+      <c r="C120" t="s">
+        <v>37</v>
+      </c>
+      <c r="F120" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO tblNeighbors VALUES (119, 'F1-108_0', 'F1-108_1');</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>120</v>
+      </c>
+      <c r="B121" t="s">
+        <v>40</v>
+      </c>
+      <c r="C121" t="s">
+        <v>50</v>
+      </c>
+      <c r="F121" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO tblNeighbors VALUES (120, 'F1-108A_0', 'F1-108A_1');</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>121</v>
+      </c>
+      <c r="B122" t="s">
+        <v>50</v>
+      </c>
+      <c r="C122" t="s">
+        <v>51</v>
+      </c>
+      <c r="F122" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO tblNeighbors VALUES (121, 'F1-108A_1', 'F1-108B');</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>122</v>
+      </c>
+      <c r="B123" t="s">
+        <v>41</v>
+      </c>
+      <c r="C123" t="s">
+        <v>52</v>
+      </c>
+      <c r="F123" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO tblNeighbors VALUES (122, 'F1-108A_2', 'F1-108C');</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>123</v>
+      </c>
+      <c r="B124" t="s">
+        <v>42</v>
+      </c>
+      <c r="C124" t="s">
+        <v>65</v>
+      </c>
+      <c r="F124" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO tblNeighbors VALUES (123, 'F1-108A_3', 'F1-T1');</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>124</v>
+      </c>
+      <c r="B125" t="s">
+        <v>43</v>
+      </c>
+      <c r="C125" t="s">
+        <v>53</v>
+      </c>
+      <c r="F125" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO tblNeighbors VALUES (124, 'F1-108A_4', 'F1-108D');</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>125</v>
+      </c>
+      <c r="B126" t="s">
+        <v>44</v>
+      </c>
+      <c r="C126" t="s">
+        <v>54</v>
+      </c>
+      <c r="F126" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO tblNeighbors VALUES (125, 'F1-108A_5', 'F1-108E');</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>126</v>
+      </c>
+      <c r="B127" t="s">
+        <v>45</v>
+      </c>
+      <c r="C127" t="s">
+        <v>61</v>
+      </c>
+      <c r="F127" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO tblNeighbors VALUES (126, 'F1-108A_6', 'F1-108L');</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>127</v>
+      </c>
+      <c r="B128" t="s">
+        <v>46</v>
+      </c>
+      <c r="C128" t="s">
+        <v>55</v>
+      </c>
+      <c r="F128" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO tblNeighbors VALUES (127, 'F1-108A_7', 'F1-108F');</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>128</v>
+      </c>
+      <c r="B129" t="s">
+        <v>47</v>
+      </c>
+      <c r="C129" t="s">
+        <v>60</v>
+      </c>
+      <c r="F129" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO tblNeighbors VALUES (128, 'F1-108A_8', 'F1-108K');</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>129</v>
+      </c>
+      <c r="B130" t="s">
+        <v>48</v>
+      </c>
+      <c r="C130" t="s">
+        <v>59</v>
+      </c>
+      <c r="F130" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO tblNeighbors VALUES (129, 'F1-108A_9', 'F1-108J');</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>130</v>
+      </c>
+      <c r="B131" t="s">
+        <v>49</v>
+      </c>
+      <c r="C131" t="s">
+        <v>57</v>
+      </c>
+      <c r="F131" t="str">
+        <f t="shared" ref="F131:F143" si="2">E$1 &amp; A131 &amp; ", '" &amp; B131 &amp; "', '" &amp; C131 &amp; "');"</f>
+        <v>INSERT INTO tblNeighbors VALUES (130, 'F1-108A_10', 'F1-108H');</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>131</v>
+      </c>
+      <c r="B132" t="s">
         <v>101</v>
       </c>
-      <c r="C118" t="s">
+      <c r="C132" t="s">
+        <v>105</v>
+      </c>
+      <c r="F132" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO tblNeighbors VALUES (131, 'F2-C1_1', 'F2-LAB');</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>132</v>
+      </c>
+      <c r="B133" t="s">
+        <v>102</v>
+      </c>
+      <c r="C133" t="s">
+        <v>101</v>
+      </c>
+      <c r="F133" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO tblNeighbors VALUES (132, 'F2-C1_0', 'F2-C1_1');</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>133</v>
+      </c>
+      <c r="B134" t="s">
+        <v>109</v>
+      </c>
+      <c r="C134" t="s">
+        <v>120</v>
+      </c>
+      <c r="F134" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO tblNeighbors VALUES (133, 'F2-LAB_2', 'F2-LAB_R');</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>134</v>
+      </c>
+      <c r="B135" t="s">
+        <v>110</v>
+      </c>
+      <c r="C135" t="s">
+        <v>118</v>
+      </c>
+      <c r="F135" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO tblNeighbors VALUES (134, 'F2-LAB_3', 'F2-LAB_F');</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>135</v>
+      </c>
+      <c r="B136" t="s">
+        <v>111</v>
+      </c>
+      <c r="C136" t="s">
+        <v>122</v>
+      </c>
+      <c r="F136" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO tblNeighbors VALUES (135, 'F2-LAB_4', 'F2-CL2');</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>136</v>
+      </c>
+      <c r="B137" t="s">
+        <v>112</v>
+      </c>
+      <c r="C137" t="s">
+        <v>121</v>
+      </c>
+      <c r="F137" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO tblNeighbors VALUES (136, 'F2-LAB_5', 'F2-R2');</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>137</v>
+      </c>
+      <c r="B138" t="s">
+        <v>119</v>
+      </c>
+      <c r="C138" t="s">
+        <v>116</v>
+      </c>
+      <c r="F138" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO tblNeighbors VALUES (137, 'F2-LAB_B0', 'F2-LAB_D');</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>138</v>
+      </c>
+      <c r="B139" t="s">
+        <v>19</v>
+      </c>
+      <c r="C139" t="s">
+        <v>21</v>
+      </c>
+      <c r="F139" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO tblNeighbors VALUES (138, 'F1-C2_0', 'F1-C2_1');</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>139</v>
+      </c>
+      <c r="B140" t="s">
+        <v>41</v>
+      </c>
+      <c r="C140" t="s">
+        <v>73</v>
+      </c>
+      <c r="F140" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO tblNeighbors VALUES (139, 'F1-108A_2', 'F1-108O');</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>140</v>
+      </c>
+      <c r="B141" t="s">
+        <v>43</v>
+      </c>
+      <c r="C141" t="s">
+        <v>66</v>
+      </c>
+      <c r="F141" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO tblNeighbors VALUES (140, 'F1-108A_4', 'F1-T2');</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>141</v>
+      </c>
+      <c r="B142" t="s">
+        <v>48</v>
+      </c>
+      <c r="C142" t="s">
+        <v>56</v>
+      </c>
+      <c r="F142" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO tblNeighbors VALUES (141, 'F1-108A_9', 'F1-108G');</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>142</v>
+      </c>
+      <c r="B143" t="s">
+        <v>101</v>
+      </c>
+      <c r="C143" t="s">
         <v>106</v>
       </c>
-      <c r="F118" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO tblNeighbors VALUES (117, 'F2-C1_1', 'F2-XR');</v>
+      <c r="F143" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO tblNeighbors VALUES (142, 'F2-C1_1', 'F2-XR');</v>
       </c>
     </row>
   </sheetData>
@@ -8356,12 +8792,109 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E2" t="str">
+        <f>D$1 &amp; A2 &amp; ", '" &amp; B2 &amp; "', '" &amp; C2 &amp; "');"</f>
+        <v>INSERT INTO tblInterFloor VALUES (1, 'F1-EL', 'F2-EL');</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E5" si="0">D$1 &amp; A3 &amp; ", '" &amp; B3 &amp; "', '" &amp; C3 &amp; "');"</f>
+        <v>INSERT INTO tblInterFloor VALUES (2, 'F2-EL', 'F1-EL');</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO tblInterFloor VALUES (3, 'F1-S2', 'F2-S2');</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO tblInterFloor VALUES (4, 'F2-S2', 'F1-S2');</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>